<commit_message>
Deleted modified documents from experiments directory
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@822 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="201">
   <si>
     <t>ID</t>
   </si>
@@ -597,10 +597,28 @@
     <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc</t>
   </si>
   <si>
-    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
-  </si>
-  <si>
     <t>4.2.RCP8.5;         5.3.ESMRCP8.5; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice</t>
+  </si>
+  <si>
+    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice</t>
+  </si>
+  <si>
+    <t>bc.062</t>
+  </si>
+  <si>
+    <t>bc.063</t>
+  </si>
+  <si>
+    <t>Prescribed SST anomolies (relative to exp 3.3) based on either (a) climatology difference between years 2026-2035 (from expt 4.1) and years 1979-2008) (from expt 3.2), OR (b) climatology difference between years 2026-2035 (from expt 1.2) and years 1979-2008 (from expt1.1)</t>
+  </si>
+  <si>
+    <t>2.1_FutureTimeSlice</t>
+  </si>
+  <si>
+    <t>Prescribed Sea Ice anomolies (relative to exp 3.3) based on either (a) climatology difference between years 2026-2035 (from expt 4.1) and years 1979-2008) (from expt 3.2), OR (b) climatology difference between years 2026-2035 (from expt 1.2) and years 1979-2008 (from expt1.1)</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G83"/>
+  <dimension ref="B2:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1095,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="80.25" customHeight="1">
@@ -1655,7 +1673,7 @@
         <v>72</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="90" customHeight="1">
@@ -1669,7 +1687,7 @@
         <v>72</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="45">
@@ -1683,7 +1701,7 @@
         <v>72</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="45">
@@ -1697,7 +1715,7 @@
         <v>72</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="79.5" customHeight="1">
@@ -1711,7 +1729,7 @@
         <v>72</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="45">
@@ -1725,7 +1743,7 @@
         <v>72</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="45">
@@ -1739,7 +1757,7 @@
         <v>72</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="45">
@@ -1753,10 +1771,10 @@
         <v>72</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="67.5" customHeight="1">
       <c r="B55" s="8" t="s">
         <v>81</v>
       </c>
@@ -1767,10 +1785,10 @@
         <v>72</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="53.25" customHeight="1">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="69.75" customHeight="1">
       <c r="B56" s="8" t="s">
         <v>82</v>
       </c>
@@ -1781,7 +1799,7 @@
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="30">
@@ -2133,6 +2151,30 @@
         <v>183</v>
       </c>
       <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="2:5" ht="78.75" customHeight="1">
+      <c r="B84" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="2:5" ht="60">
+      <c r="B85" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E85" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Most recent conformance spreadsheet uploaded
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@825 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="218">
   <si>
     <t>ID</t>
   </si>
@@ -447,9 +447,6 @@
     <t>6.2a.HansenBaseline</t>
   </si>
   <si>
-    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2</t>
-  </si>
-  <si>
     <t>bc.055</t>
   </si>
   <si>
@@ -510,9 +507,6 @@
     <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl</t>
   </si>
   <si>
-    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl</t>
-  </si>
-  <si>
     <t>ic.008</t>
   </si>
   <si>
@@ -591,21 +585,9 @@
     <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit</t>
   </si>
   <si>
-    <t>3.3.AMIP; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc</t>
-  </si>
-  <si>
-    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc</t>
-  </si>
-  <si>
     <t>4.2.RCP8.5;         5.3.ESMRCP8.5; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
   </si>
   <si>
-    <t>3.1S_100yrControl, 2.1_FutureTimeSlice</t>
-  </si>
-  <si>
-    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice</t>
-  </si>
-  <si>
     <t>bc.062</t>
   </si>
   <si>
@@ -619,6 +601,75 @@
   </si>
   <si>
     <t>Prescribed Sea Ice anomolies (relative to exp 3.3) based on either (a) climatology difference between years 2026-2035 (from expt 4.1) and years 1979-2008) (from expt 3.2), OR (b) climatology difference between years 2026-2035 (from expt 1.2) and years 1979-2008 (from expt1.1)</t>
+  </si>
+  <si>
+    <t>3.3E_AMIP_Ensemble</t>
+  </si>
+  <si>
+    <t>ic.015</t>
+  </si>
+  <si>
+    <t>ic.016</t>
+  </si>
+  <si>
+    <t>Alternate initial conditions imposed on the atmosphere (compared to the control run 3.3)</t>
+  </si>
+  <si>
+    <t>Alternate initial conditions imposed on the land (compared to the control run 3.3)</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble</t>
+  </si>
+  <si>
+    <t>ic.017</t>
+  </si>
+  <si>
+    <t>ic.018</t>
+  </si>
+  <si>
+    <t>ic.019</t>
+  </si>
+  <si>
+    <t>ic.020</t>
+  </si>
+  <si>
+    <t>Different initial conditions imposed on atmosphere to that of experiment 2.1</t>
+  </si>
+  <si>
+    <t>2.1E_FutureTimeSlice_Ensemble</t>
+  </si>
+  <si>
+    <t>Different initial conditions imposed on ocean to that of experiment 2.1</t>
+  </si>
+  <si>
+    <t>Different initial conditions imposed on sea-ice to that of experiment 2.1</t>
+  </si>
+  <si>
+    <t>Different initial conditions imposed on land surface to that of experiment 2.1</t>
+  </si>
+  <si>
+    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice; 2.1E_FutureTimeSlice_Ensemble</t>
+  </si>
+  <si>
+    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2</t>
+  </si>
+  <si>
+    <t>6.3.GregoryAbrupt4XCO2; 6.5.CloudResponse.4CO2</t>
+  </si>
+  <si>
+    <t>6.2b.Hansen4XCO2.xml; 6.5.CloudResponse.4CO2</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl; 6.5.CloudResponse.4CO2</t>
+  </si>
+  <si>
+    <t>3.3E_AMIP_Ensemble; 6.5.CloudResponse.4CO2</t>
   </si>
 </sst>
 </file>
@@ -740,7 +791,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -766,6 +817,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1062,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G85"/>
+  <dimension ref="B2:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1073,7 +1127,7 @@
     <col min="1" max="1" width="10.42578125" style="4"/>
     <col min="2" max="2" width="21.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="68.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="4" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="68.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="4"/>
     <col min="7" max="7" width="38.85546875" style="1" customWidth="1"/>
@@ -1102,21 +1156,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="33" customHeight="1" thickTop="1">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="80.25" customHeight="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="30">
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1127,7 +1181,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>143</v>
+        <v>213</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -1143,7 +1197,9 @@
       <c r="D6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="8" t="s">
@@ -1173,1008 +1229,1082 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="2:7" ht="30">
+      <c r="B10" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="2:7" ht="84.75" customHeight="1">
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1">
       <c r="B11" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:7" ht="30">
       <c r="B12" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="D12" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="2:7" ht="30">
       <c r="B14" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="2:7" ht="45">
       <c r="B16" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B21" s="3" t="s">
+    <row r="18" spans="2:7" ht="30">
+      <c r="B18" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:7" ht="30">
+      <c r="B19" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:7" ht="30">
+      <c r="B20" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:7" s="1" customFormat="1" ht="32.25" customHeight="1">
+      <c r="B21" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:7" ht="36" customHeight="1">
+      <c r="B22" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:7" ht="30">
+      <c r="B23" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="14"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="14"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B22" s="7" t="s">
+    <row r="27" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B27" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30.75" thickTop="1">
-      <c r="B23" s="8" t="s">
+    <row r="28" spans="2:7" ht="30.75" thickTop="1">
+      <c r="B28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30">
-      <c r="B24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30">
-      <c r="B25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30">
-      <c r="B27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30">
-      <c r="B28" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30">
       <c r="B29" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30">
       <c r="B30" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30">
       <c r="B32" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="60.75" customHeight="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30">
       <c r="B33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30">
+      <c r="B35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30">
+      <c r="B36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30">
+      <c r="B37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="60.75" customHeight="1">
+      <c r="B38" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="74.25" customHeight="1">
-      <c r="B34" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="88.5" customHeight="1">
-      <c r="B35" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="67.5" customHeight="1">
-      <c r="B36" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="80.25" customHeight="1">
-      <c r="B37" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="81" customHeight="1">
-      <c r="B38" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="69" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="74.25" customHeight="1">
       <c r="B39" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="113.25" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="88.5" customHeight="1">
       <c r="B40" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="105.75" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="67.5" customHeight="1">
       <c r="B41" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="81" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="80.25" customHeight="1">
       <c r="B42" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="90.75" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="81" customHeight="1">
       <c r="B43" s="8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="70.5" customHeight="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="69" customHeight="1">
       <c r="B44" s="8" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="113.25" customHeight="1">
       <c r="B45" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="105.75" customHeight="1">
+      <c r="B46" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="81" customHeight="1">
+      <c r="B47" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="90.75" customHeight="1">
+      <c r="B48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="70.5" customHeight="1">
+      <c r="B49" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D50" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="8" t="s">
+      <c r="E50" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D51" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="2:5" ht="45">
-      <c r="B47" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="90" customHeight="1">
-      <c r="B48" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="45">
-      <c r="B49" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="45">
-      <c r="B50" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="79.5" customHeight="1">
-      <c r="B51" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>72</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="45">
+    <row r="52" spans="2:5" ht="60">
       <c r="B52" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="90" customHeight="1">
       <c r="B53" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="60">
       <c r="B54" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="67.5" customHeight="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="60">
       <c r="B55" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="69.75" customHeight="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="79.5" customHeight="1">
       <c r="B56" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="30">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="60">
       <c r="B57" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="60">
+      <c r="B58" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="60">
+      <c r="B59" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="67.5" customHeight="1">
+      <c r="B60" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="69.75" customHeight="1">
+      <c r="B61" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="30">
+      <c r="B62" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="B60" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="B62" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>114</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="E63" s="6"/>
     </row>
     <row r="64" spans="2:5">
       <c r="B64" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>131</v>
-      </c>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="2:5">
       <c r="B65" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="30">
-      <c r="B66" s="8" t="s">
+    <row r="71" spans="2:5" ht="30">
+      <c r="B71" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D71" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="2:5" ht="30">
-      <c r="B67" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="2:5" ht="30">
-      <c r="B68" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="2:5" ht="30">
-      <c r="B69" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="2:5" ht="30">
-      <c r="B70" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>121</v>
-      </c>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" spans="2:5" ht="30">
       <c r="B72" s="8" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>121</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" spans="2:5" ht="30">
       <c r="B73" s="8" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="2:5">
+    <row r="74" spans="2:5" ht="30">
       <c r="B74" s="8" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5">
+        <v>121</v>
+      </c>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="2:5" ht="30">
       <c r="B75" s="8" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" ht="30">
+        <v>125</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="2:5">
       <c r="B76" s="8" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>141</v>
+        <v>60</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="30">
       <c r="B77" s="8" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>145</v>
+        <v>62</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E77" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="78" spans="2:5" ht="30">
       <c r="B78" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="30">
+      <c r="B81" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="30">
+      <c r="B82" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="2:5" ht="30">
+      <c r="B83" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="D83" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="63.75" customHeight="1">
-      <c r="B79" s="8" t="s">
+      <c r="E83" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="63.75" customHeight="1">
+      <c r="B84" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="D84" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="55.5" customHeight="1">
+      <c r="B85" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="C85" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5">
+      <c r="B86" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="2:5">
+      <c r="B88" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="2:5" ht="78.75" customHeight="1">
+      <c r="B89" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="E79" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="55.5" customHeight="1">
-      <c r="B80" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5">
-      <c r="B81" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E81" s="6"/>
-    </row>
-    <row r="82" spans="2:5">
-      <c r="B82" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E82" s="6"/>
-    </row>
-    <row r="83" spans="2:5">
-      <c r="B83" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E83" s="6"/>
-    </row>
-    <row r="84" spans="2:5" ht="78.75" customHeight="1">
-      <c r="B84" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E84" s="6"/>
-    </row>
-    <row r="85" spans="2:5" ht="60">
-      <c r="B85" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E85" s="6"/>
+      <c r="C89" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="60">
+      <c r="B90" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added most recent updated Conformance Crossover spreadsheet
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@836 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="240">
   <si>
     <t>ID</t>
   </si>
@@ -618,15 +618,6 @@
     <t>Alternate initial conditions imposed on the land (compared to the control run 3.3)</t>
   </si>
   <si>
-    <t>3.3.AMIP; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble</t>
-  </si>
-  <si>
-    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble</t>
-  </si>
-  <si>
-    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble</t>
-  </si>
-  <si>
     <t>ic.017</t>
   </si>
   <si>
@@ -657,9 +648,6 @@
     <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice; 2.1E_FutureTimeSlice_Ensemble</t>
   </si>
   <si>
-    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2</t>
-  </si>
-  <si>
     <t>6.3.GregoryAbrupt4XCO2; 6.5.CloudResponse.4CO2</t>
   </si>
   <si>
@@ -670,6 +658,84 @@
   </si>
   <si>
     <t>3.3E_AMIP_Ensemble; 6.5.CloudResponse.4CO2</t>
+  </si>
+  <si>
+    <t>3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST</t>
+  </si>
+  <si>
+    <t>ic.021</t>
+  </si>
+  <si>
+    <t>bc.064</t>
+  </si>
+  <si>
+    <t>Patterned SST perturbation applied to the AMIP SSTs of expt 3.3 (provided by CFMIP)</t>
+  </si>
+  <si>
+    <t>6.6.CloudResponse.SST</t>
+  </si>
+  <si>
+    <t>bc.065</t>
+  </si>
+  <si>
+    <t>Imposed zonally uniform SSTs on an aquaplanet</t>
+  </si>
+  <si>
+    <t>6.7a.Aquaplanet_Control</t>
+  </si>
+  <si>
+    <t>bc.066</t>
+  </si>
+  <si>
+    <t>Imposed 4*CO2 on the control experiment 6.7a</t>
+  </si>
+  <si>
+    <t>6.7b_Aquaplanet_4CO2</t>
+  </si>
+  <si>
+    <t>bc.067</t>
+  </si>
+  <si>
+    <t>Imposed +4K on the uniform SSTs of controlexperiment 6.7a</t>
+  </si>
+  <si>
+    <t>6.7c_Aquaplanet_4K</t>
+  </si>
+  <si>
+    <t>6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K</t>
+  </si>
+  <si>
+    <t>bc.068</t>
+  </si>
+  <si>
+    <t>Imposed +4K on the SSTs of controlexperiment 3.3</t>
+  </si>
+  <si>
+    <t>6.8.Cloudresponse.UniSST</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST</t>
+  </si>
+  <si>
+    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2; 3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>Additional runs, initialised at different points in the control run</t>
+  </si>
+  <si>
+    <t>3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>5.2.ESMHistoricalC20th; 3.2E_HistoricalEnsemble</t>
   </si>
 </sst>
 </file>
@@ -1116,9 +1182,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G90"/>
+  <dimension ref="B2:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
@@ -1156,7 +1222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" ht="33" customHeight="1" thickTop="1">
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="64.5" customHeight="1" thickTop="1">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1167,10 +1233,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="30">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="38.25" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1181,13 +1247,13 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" ht="23.25" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>63</v>
       </c>
@@ -1198,7 +1264,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -1363,137 +1429,116 @@
     </row>
     <row r="20" spans="2:7" ht="30">
       <c r="B20" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:7" s="1" customFormat="1" ht="32.25" customHeight="1">
       <c r="B21" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="36" customHeight="1">
       <c r="B22" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="30">
       <c r="B23" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="14"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="14"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="10"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="2:7">
+      <c r="B26" s="14"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="14"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="14"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B27" s="7" t="s">
+    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B30" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30.75" thickTop="1">
-      <c r="B28" s="8" t="s">
+    <row r="31" spans="2:7" ht="30.75" thickTop="1">
+      <c r="B31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30">
-      <c r="B29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30">
-      <c r="B30" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>6</v>
@@ -1501,27 +1546,30 @@
       <c r="E31" s="6" t="s">
         <v>160</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="32" spans="2:7" ht="30">
       <c r="B32" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30">
       <c r="B33" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>6</v>
@@ -1529,447 +1577,453 @@
       <c r="E33" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30">
       <c r="B35" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30">
       <c r="B36" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30">
+    <row r="37" spans="2:7">
       <c r="B37" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="60.75" customHeight="1">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30">
       <c r="B38" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30">
+      <c r="B39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30">
+      <c r="B40" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="119.25" customHeight="1">
+      <c r="B41" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="74.25" customHeight="1">
-      <c r="B39" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="88.5" customHeight="1">
-      <c r="B40" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="67.5" customHeight="1">
-      <c r="B41" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="80.25" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="123" customHeight="1">
       <c r="B42" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="81" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="120" customHeight="1">
       <c r="B43" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="69" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="120.75" customHeight="1">
       <c r="B44" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="113.25" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="111.75" customHeight="1">
       <c r="B45" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="105.75" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="138" customHeight="1">
       <c r="B46" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" ht="81" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="138" customHeight="1">
       <c r="B47" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="90.75" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="117.75" customHeight="1">
       <c r="B48" s="8" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="70.5" customHeight="1">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="114.75" customHeight="1">
       <c r="B49" s="8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="110.25" customHeight="1">
       <c r="B50" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="108.75" customHeight="1">
+      <c r="B51" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="101.25" customHeight="1">
+      <c r="B52" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="44.25" customHeight="1">
+      <c r="B53" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="8" t="s">
+      <c r="E53" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="39.75" customHeight="1">
+      <c r="B54" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="60">
-      <c r="B52" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="90" customHeight="1">
-      <c r="B53" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="60">
-      <c r="B54" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="E54" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="60">
       <c r="B55" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="79.5" customHeight="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="90" customHeight="1">
       <c r="B56" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="60">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="71.25" customHeight="1">
       <c r="B57" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="60">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="75" customHeight="1">
       <c r="B58" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="60">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="79.5" customHeight="1">
       <c r="B59" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="67.5" customHeight="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="60">
       <c r="B60" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="69.75" customHeight="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="75.75" customHeight="1">
       <c r="B61" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E61" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="60">
+      <c r="B62" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="67.5" customHeight="1">
+      <c r="B63" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="69.75" customHeight="1">
+      <c r="B64" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="30">
-      <c r="B62" s="8" t="s">
+    <row r="65" spans="2:5" ht="30">
+      <c r="B65" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="2:5">
-      <c r="B63" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="B64" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="2:5">
-      <c r="B65" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>93</v>
@@ -1978,333 +2032,431 @@
     </row>
     <row r="66" spans="2:5">
       <c r="B66" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E66" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="E67" s="6"/>
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E68" s="6" t="s">
-        <v>130</v>
-      </c>
+      <c r="E68" s="6"/>
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="71" spans="2:5" ht="30">
-      <c r="B71" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="72" spans="2:5" ht="30">
-      <c r="B72" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="2:5" ht="30">
-      <c r="B73" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E73" s="6"/>
     </row>
     <row r="74" spans="2:5" ht="30">
       <c r="B74" s="8" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="E74" s="6"/>
     </row>
     <row r="75" spans="2:5" ht="30">
       <c r="B75" s="8" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="2:5">
+    <row r="76" spans="2:5" ht="30">
       <c r="B76" s="8" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>121</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E76" s="6"/>
     </row>
     <row r="77" spans="2:5" ht="30">
       <c r="B77" s="8" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E77" s="6" t="s">
         <v>121</v>
       </c>
+      <c r="E77" s="6"/>
     </row>
     <row r="78" spans="2:5" ht="30">
       <c r="B78" s="8" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="E78" s="6"/>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="8" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>139</v>
+        <v>60</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="30">
       <c r="B80" s="8" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="30">
       <c r="B81" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="30">
+        <v>134</v>
+      </c>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="2:5">
       <c r="B82" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E82" s="6"/>
-    </row>
-    <row r="83" spans="2:5" ht="30">
+      <c r="E82" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
       <c r="B83" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="30">
+      <c r="B84" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="30">
+      <c r="B85" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="2:5" ht="30">
+      <c r="B86" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D86" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="63.75" customHeight="1">
-      <c r="B84" s="8" t="s">
+      <c r="E86" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="63.75" customHeight="1">
+      <c r="B87" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D87" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="55.5" customHeight="1">
-      <c r="B85" s="8" t="s">
+    <row r="88" spans="2:5" ht="55.5" customHeight="1">
+      <c r="B88" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D88" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E88" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="2:5">
-      <c r="B86" s="8" t="s">
+    <row r="89" spans="2:5">
+      <c r="B89" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D89" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E86" s="6"/>
-    </row>
-    <row r="87" spans="2:5">
-      <c r="B87" s="8" t="s">
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D90" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E87" s="6"/>
-    </row>
-    <row r="88" spans="2:5">
-      <c r="B88" s="8" t="s">
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="B91" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D91" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E88" s="6"/>
-    </row>
-    <row r="89" spans="2:5" ht="78.75" customHeight="1">
-      <c r="B89" s="8" t="s">
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="2:5" ht="78.75" customHeight="1">
+      <c r="B92" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D92" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E89" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="60">
-      <c r="B90" s="8" t="s">
+      <c r="E92" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="60">
+      <c r="B93" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D93" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E90" s="6" t="s">
-        <v>208</v>
-      </c>
+      <c r="E93" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="30">
+      <c r="B94" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5">
+      <c r="B96" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="2:5">
+      <c r="B97" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="2:5">
+      <c r="B98" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="E98" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated paleo conformance docs and updated spreadsheet
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@838 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="259">
   <si>
     <t>ID</t>
   </si>
@@ -714,9 +714,6 @@
     <t>6.8.Cloudresponse.UniSST</t>
   </si>
   <si>
-    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST</t>
-  </si>
-  <si>
     <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2; 3.2E_HistoricalEnsemble</t>
   </si>
   <si>
@@ -736,6 +733,66 @@
   </si>
   <si>
     <t>5.2.ESMHistoricalC20th; 3.2E_HistoricalEnsemble</t>
+  </si>
+  <si>
+    <t>bc.069</t>
+  </si>
+  <si>
+    <t>3.4_MidHolocene</t>
+  </si>
+  <si>
+    <t>bc.070</t>
+  </si>
+  <si>
+    <t>Impose Mid-Holocene orbital parameter conditions</t>
+  </si>
+  <si>
+    <t>Impose Mid-Holocene conditions of well-mixed gases</t>
+  </si>
+  <si>
+    <t>bc.071</t>
+  </si>
+  <si>
+    <t>Impose Mid-Holocene solar forcing conditions</t>
+  </si>
+  <si>
+    <t>ic.022</t>
+  </si>
+  <si>
+    <t>bc.072</t>
+  </si>
+  <si>
+    <t>bc.073</t>
+  </si>
+  <si>
+    <t>Impose last glacial maximum conditions of well-mixed gases</t>
+  </si>
+  <si>
+    <t>3.5_Last_Glacial_Max</t>
+  </si>
+  <si>
+    <t>Ocean initialised from a cold spun-up state provided by PMIP</t>
+  </si>
+  <si>
+    <t>Impose last glacial maximum ice sheet conditions supplied by PMIP</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.4_MidHolocene; 3.5_Last_Glacial_Max; 3.6_Last_Millennium</t>
+  </si>
+  <si>
+    <t>bc.074</t>
+  </si>
+  <si>
+    <t>bc.075</t>
+  </si>
+  <si>
+    <t>3.6_Last_Millennium</t>
+  </si>
+  <si>
+    <t>Impose evolving volcanic aerosol conditions consistant with PMIP requirements</t>
+  </si>
+  <si>
+    <t>Impose evolving solar conditions consistant with PMIP requirements</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G98"/>
+  <dimension ref="B2:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1222,7 +1279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" ht="64.5" customHeight="1" thickTop="1">
+    <row r="4" spans="2:7" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1233,10 +1290,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="38.25" customHeight="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="53.25" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1247,13 +1304,13 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="23.25" customHeight="1">
+    <row r="6" spans="2:7" ht="33" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>63</v>
       </c>
@@ -1267,7 +1324,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" ht="21.75" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>70</v>
       </c>
@@ -1281,7 +1338,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" ht="28.5" customHeight="1">
       <c r="B8" s="8" t="s">
         <v>103</v>
       </c>
@@ -1293,7 +1350,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" ht="30.75" customHeight="1">
       <c r="B9" s="8" t="s">
         <v>148</v>
       </c>
@@ -1305,7 +1362,7 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="2:7" ht="30">
+    <row r="10" spans="2:7" ht="42" customHeight="1">
       <c r="B10" s="8" t="s">
         <v>151</v>
       </c>
@@ -1480,29 +1537,35 @@
         <v>215</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>235</v>
-      </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="14"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="B25" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="14"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="2:7">
       <c r="B27" s="14"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="2:7">
@@ -1511,79 +1574,71 @@
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B29" s="3" t="s">
+    <row r="29" spans="2:7">
+      <c r="B29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B30" s="7" t="s">
+    <row r="31" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B31" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30.75" thickTop="1">
-      <c r="B31" s="8" t="s">
+    <row r="32" spans="2:7" ht="30.75" thickTop="1">
+      <c r="B32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30">
-      <c r="B32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30">
       <c r="B33" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30">
       <c r="B34" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>6</v>
@@ -1592,12 +1647,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30">
+    <row r="35" spans="2:7">
       <c r="B35" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>6</v>
@@ -1608,10 +1663,10 @@
     </row>
     <row r="36" spans="2:7" ht="30">
       <c r="B36" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>6</v>
@@ -1619,30 +1674,30 @@
       <c r="E36" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7">
+    </row>
+    <row r="37" spans="2:7" ht="30">
       <c r="B37" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30">
+        <v>160</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
       <c r="B38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>6</v>
@@ -1653,10 +1708,10 @@
     </row>
     <row r="39" spans="2:7" ht="30">
       <c r="B39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>6</v>
@@ -1664,240 +1719,240 @@
       <c r="E39" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="40" spans="2:7" ht="30">
       <c r="B40" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="30">
+      <c r="B41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="119.25" customHeight="1">
-      <c r="B41" s="8" t="s">
+    <row r="42" spans="2:7" ht="119.25" customHeight="1">
+      <c r="B42" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="123" customHeight="1">
-      <c r="B42" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="120" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="123" customHeight="1">
       <c r="B43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="120.75" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="120" customHeight="1">
       <c r="B44" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="111.75" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="120.75" customHeight="1">
       <c r="B45" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" ht="138" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="111.75" customHeight="1">
       <c r="B46" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="138" customHeight="1">
       <c r="B47" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="117.75" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="138" customHeight="1">
       <c r="B48" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="114.75" customHeight="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="117.75" customHeight="1">
       <c r="B49" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="110.25" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="114.75" customHeight="1">
       <c r="B50" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="108.75" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="110.25" customHeight="1">
       <c r="B51" s="8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="101.25" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="108.75" customHeight="1">
       <c r="B52" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="44.25" customHeight="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="101.25" customHeight="1">
       <c r="B53" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="44.25" customHeight="1">
+      <c r="B54" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="39.75" customHeight="1">
-      <c r="B54" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="39.75" customHeight="1">
+      <c r="B55" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="60">
-      <c r="B55" s="8" t="s">
+    <row r="56" spans="2:5" ht="60">
+      <c r="B56" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="90" customHeight="1">
-      <c r="B56" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>72</v>
@@ -1906,12 +1961,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="71.25" customHeight="1">
+    <row r="57" spans="2:5" ht="90" customHeight="1">
       <c r="B57" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>72</v>
@@ -1920,12 +1975,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="75" customHeight="1">
+    <row r="58" spans="2:5" ht="71.25" customHeight="1">
       <c r="B58" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>72</v>
@@ -1934,12 +1989,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="79.5" customHeight="1">
+    <row r="59" spans="2:5" ht="75" customHeight="1">
       <c r="B59" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>72</v>
@@ -1948,12 +2003,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="60">
+    <row r="60" spans="2:5" ht="79.5" customHeight="1">
       <c r="B60" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>72</v>
@@ -1962,12 +2017,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="75.75" customHeight="1">
+    <row r="61" spans="2:5" ht="60">
       <c r="B61" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>72</v>
@@ -1976,12 +2031,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="60">
+    <row r="62" spans="2:5" ht="75.75" customHeight="1">
       <c r="B62" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>72</v>
@@ -1990,12 +2045,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="67.5" customHeight="1">
+    <row r="63" spans="2:5" ht="60">
       <c r="B63" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>72</v>
@@ -2004,38 +2059,40 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="69.75" customHeight="1">
+    <row r="64" spans="2:5" ht="67.5" customHeight="1">
       <c r="B64" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>72</v>
       </c>
       <c r="E64" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="69.75" customHeight="1">
+      <c r="B65" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="30">
-      <c r="B65" s="8" t="s">
+    <row r="66" spans="2:5" ht="30">
+      <c r="B66" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>93</v>
@@ -2044,10 +2101,10 @@
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>93</v>
@@ -2056,10 +2113,10 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>93</v>
@@ -2068,92 +2125,92 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>128</v>
-      </c>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="2:5">
       <c r="B71" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="2:5">
       <c r="B72" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="2:5">
       <c r="B73" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E73" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="74" spans="2:5" ht="30">
-      <c r="B74" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="6"/>
     </row>
     <row r="75" spans="2:5" ht="30">
       <c r="B75" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>105</v>
@@ -2162,10 +2219,10 @@
     </row>
     <row r="76" spans="2:5" ht="30">
       <c r="B76" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>105</v>
@@ -2174,102 +2231,100 @@
     </row>
     <row r="77" spans="2:5" ht="30">
       <c r="B77" s="8" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="E77" s="6"/>
     </row>
     <row r="78" spans="2:5" ht="30">
       <c r="B78" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="2:5" ht="30">
+      <c r="B79" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="2:5">
-      <c r="B79" s="8" t="s">
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="30">
-      <c r="B80" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="30">
       <c r="B81" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="30">
+      <c r="B82" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D82" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="6"/>
-    </row>
-    <row r="82" spans="2:5">
-      <c r="B82" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="E82" s="6"/>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>142</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="30">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
       <c r="B84" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>142</v>
@@ -2280,50 +2335,50 @@
     </row>
     <row r="85" spans="2:5" ht="30">
       <c r="B85" s="8" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E85" s="6"/>
+      <c r="E85" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="86" spans="2:5" ht="30">
       <c r="B86" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="2:5" ht="30">
+      <c r="B87" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="D87" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E87" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="63.75" customHeight="1">
-      <c r="B87" s="8" t="s">
+    <row r="88" spans="2:5" ht="63.75" customHeight="1">
+      <c r="B88" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="55.5" customHeight="1">
-      <c r="B88" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>188</v>
@@ -2332,62 +2387,62 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="2:5">
+    <row r="89" spans="2:5" ht="55.5" customHeight="1">
       <c r="B89" s="8" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E89" s="6"/>
+        <v>188</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="2:5">
+      <c r="B92" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C92" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D92" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="2:5" ht="78.75" customHeight="1">
-      <c r="B92" s="8" t="s">
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="2:5" ht="78.75" customHeight="1">
+      <c r="B93" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" ht="60">
-      <c r="B93" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>193</v>
@@ -2396,67 +2451,165 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="2:5" ht="30">
+    <row r="94" spans="2:5" ht="60">
       <c r="B94" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="30">
+      <c r="B95" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C95" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="D95" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="E94" s="6"/>
-    </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>228</v>
-      </c>
+      <c r="E95" s="6"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E96" s="6"/>
+        <v>221</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="2:5">
+      <c r="B99" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C99" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D99" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="E98" s="6"/>
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="2:5">
+      <c r="B100" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="2:5">
+      <c r="B101" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="2:5">
+      <c r="B102" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E102" s="6"/>
+    </row>
+    <row r="103" spans="2:5">
+      <c r="B103" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="2:5">
+      <c r="B104" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="B105" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="2:5" ht="30">
+      <c r="B106" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E106" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added updated 'Future' experiments and updated crossover spreadsheet
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@839 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="306">
   <si>
     <t>ID</t>
   </si>
@@ -396,27 +396,9 @@
     <t>Imposed changing emissions of historical volcanic well mixed gases, including CO2</t>
   </si>
   <si>
-    <t>4.2.RCP8.5; 5.3.ESMRCP8.5</t>
-  </si>
-  <si>
     <t>Prescribed non-evolving  emissions of pre-industrial natural aerosol precursors</t>
   </si>
   <si>
-    <t>5.3.ESMRCP8.5</t>
-  </si>
-  <si>
-    <t>5.3.ESMRCP8.6</t>
-  </si>
-  <si>
-    <t>5.3.ESMRCP8.7</t>
-  </si>
-  <si>
-    <t>5.3.ESMRCP8.8</t>
-  </si>
-  <si>
-    <t>5.3.ESMRCP8.9</t>
-  </si>
-  <si>
     <t>bc.051</t>
   </si>
   <si>
@@ -585,9 +567,6 @@
     <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit</t>
   </si>
   <si>
-    <t>4.2.RCP8.5;         5.3.ESMRCP8.5; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
-  </si>
-  <si>
     <t>bc.062</t>
   </si>
   <si>
@@ -645,9 +624,6 @@
     <t>Different initial conditions imposed on land surface to that of experiment 2.1</t>
   </si>
   <si>
-    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice; 2.1E_FutureTimeSlice_Ensemble</t>
-  </si>
-  <si>
     <t>6.3.GregoryAbrupt4XCO2; 6.5.CloudResponse.4CO2</t>
   </si>
   <si>
@@ -793,6 +769,171 @@
   </si>
   <si>
     <t>Impose evolving solar conditions consistant with PMIP requirements</t>
+  </si>
+  <si>
+    <t>bc.076</t>
+  </si>
+  <si>
+    <t>bc.077</t>
+  </si>
+  <si>
+    <t>bc.078</t>
+  </si>
+  <si>
+    <t>bc.079</t>
+  </si>
+  <si>
+    <t>bc.080</t>
+  </si>
+  <si>
+    <t>bc.081</t>
+  </si>
+  <si>
+    <t>bc.082</t>
+  </si>
+  <si>
+    <t>bc.083</t>
+  </si>
+  <si>
+    <t>bc.084</t>
+  </si>
+  <si>
+    <t>bc.085</t>
+  </si>
+  <si>
+    <t>4.3.RCP2.X</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP2.X well mixed gases, including CO2</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP2.X short lived gas species</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP2.X aerosols</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP2.X aerosol precursors</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP2.X well mixed gases, including CO2</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP2.X short lived gas species</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP2.X aerosols</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP2.X aerosol precursors</t>
+  </si>
+  <si>
+    <t>Imposed changing RCP2.X land use</t>
+  </si>
+  <si>
+    <t>bc.086</t>
+  </si>
+  <si>
+    <t>bc.087</t>
+  </si>
+  <si>
+    <t>bc.088</t>
+  </si>
+  <si>
+    <t>bc.089</t>
+  </si>
+  <si>
+    <t>bc.090</t>
+  </si>
+  <si>
+    <t>bc.091</t>
+  </si>
+  <si>
+    <t>bc.092</t>
+  </si>
+  <si>
+    <t>bc.093</t>
+  </si>
+  <si>
+    <t>bc.094</t>
+  </si>
+  <si>
+    <t>bc.095</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP6 well mixed gases, including CO2</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP6 short lived gas species</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP6 aerosols</t>
+  </si>
+  <si>
+    <t>Imposed changing concentrations of RCP6 aerosol precursors</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP6 well mixed gases, including CO2</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP6 short lived gas species</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP6 aerosols</t>
+  </si>
+  <si>
+    <t>Imposed changing emissions of RCP6 aerosol precursors</t>
+  </si>
+  <si>
+    <t>Imposed changing RCP6 land use</t>
+  </si>
+  <si>
+    <t>4.4.RCP6</t>
+  </si>
+  <si>
+    <t>RCP4.5 conditions extended through year 2300</t>
+  </si>
+  <si>
+    <t>1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 2.1_FutureTimeSlice; 2.1E_FutureTimeSlice_Ensemble; 4.1L.RCP4.5_EXT</t>
+  </si>
+  <si>
+    <t>RCP8.5 conditions extended through year 2300</t>
+  </si>
+  <si>
+    <t>4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>5.3.ESMRCP8.5; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>5.3.ESMRCP8.6; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>5.3.ESMRCP8.7; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>5.3.ESMRCP8.8; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>5.3.ESMRCP8.9; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>4.2.RCP8.5;         5.3.ESMRCP8.5; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 4.3.RCP2.X; 4.4.RCP6; 4.1L.RCP4.5_EXT; ; 4.2L.RCP8.5_Ext</t>
+  </si>
+  <si>
+    <t>bc.096</t>
+  </si>
+  <si>
+    <t>RCP2.X conditions extended through year 2300</t>
+  </si>
+  <si>
+    <t>4.2.RCP8.5; 5.3.ESMRCP8.5; 4.3_RCP2.X; 4.1L.RCP4.5_EXT; 4.2L.RCP8.5_Ext; 4.3L.RCP2.X_EXT</t>
+  </si>
+  <si>
+    <t>4.3L.RCP2.X_Ext</t>
+  </si>
+  <si>
+    <t>4.1L.RCP4.5_Ext</t>
   </si>
 </sst>
 </file>
@@ -1239,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G106"/>
+  <dimension ref="B2:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1290,7 +1431,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="53.25" customHeight="1">
@@ -1304,7 +1445,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -1321,21 +1462,21 @@
         <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="21.75" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="36.75" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>126</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="28.5" customHeight="1">
@@ -1352,207 +1493,207 @@
     </row>
     <row r="9" spans="2:7" ht="30.75" customHeight="1">
       <c r="B9" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:7" ht="42" customHeight="1">
       <c r="B10" s="8" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1">
       <c r="B11" s="12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:7" ht="30">
       <c r="B12" s="12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="2:7" ht="30">
       <c r="B14" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>177</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="2:7" ht="45">
       <c r="B16" s="12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="12" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="2:7" ht="30">
       <c r="B18" s="12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="2:7" ht="30">
       <c r="B19" s="12" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="2:7" ht="30">
       <c r="B20" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:7" s="1" customFormat="1" ht="32.25" customHeight="1">
       <c r="B21" s="15" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="36" customHeight="1">
       <c r="B22" s="12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="30">
       <c r="B23" s="12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="12" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E25" s="6"/>
     </row>
@@ -1613,7 +1754,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>45</v>
@@ -1630,7 +1771,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30">
@@ -1644,7 +1785,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:7">
@@ -1658,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30">
@@ -1672,7 +1813,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="30">
@@ -1686,7 +1827,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>29</v>
@@ -1703,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30">
@@ -1711,13 +1852,13 @@
         <v>16</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30">
@@ -1731,7 +1872,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>29</v>
@@ -1748,7 +1889,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="119.25" customHeight="1">
@@ -1762,7 +1903,7 @@
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="123" customHeight="1">
@@ -1776,7 +1917,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="120" customHeight="1">
@@ -1790,7 +1931,7 @@
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="120.75" customHeight="1">
@@ -1804,7 +1945,7 @@
         <v>49</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="111.75" customHeight="1">
@@ -1818,7 +1959,7 @@
         <v>49</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="138" customHeight="1">
@@ -1832,7 +1973,7 @@
         <v>49</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="138" customHeight="1">
@@ -1846,7 +1987,7 @@
         <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="117.75" customHeight="1">
@@ -1860,7 +2001,7 @@
         <v>49</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="114.75" customHeight="1">
@@ -1874,7 +2015,7 @@
         <v>49</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="110.25" customHeight="1">
@@ -1888,7 +2029,7 @@
         <v>49</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="108.75" customHeight="1">
@@ -1902,7 +2043,7 @@
         <v>49</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="101.25" customHeight="1">
@@ -1916,7 +2057,7 @@
         <v>49</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="44.25" customHeight="1">
@@ -1930,7 +2071,7 @@
         <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="39.75" customHeight="1">
@@ -1944,7 +2085,7 @@
         <v>65</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="60">
@@ -1954,11 +2095,11 @@
       <c r="C56" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="90" customHeight="1">
@@ -1968,11 +2109,11 @@
       <c r="C57" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="2:5" ht="71.25" customHeight="1">
@@ -1982,11 +2123,11 @@
       <c r="C58" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="2:5" ht="75" customHeight="1">
@@ -1996,11 +2137,11 @@
       <c r="C59" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="79.5" customHeight="1">
@@ -2010,11 +2151,11 @@
       <c r="C60" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" spans="2:5" ht="60">
@@ -2024,11 +2165,11 @@
       <c r="C61" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="75.75" customHeight="1">
@@ -2038,11 +2179,11 @@
       <c r="C62" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="2:5" ht="60">
@@ -2052,11 +2193,11 @@
       <c r="C63" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="67.5" customHeight="1">
@@ -2066,25 +2207,25 @@
       <c r="C64" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="69.75" customHeight="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="79.5" customHeight="1">
       <c r="B65" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>189</v>
+        <v>300</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="30">
@@ -2097,7 +2238,9 @@
       <c r="D66" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E66" s="6"/>
+      <c r="E66" s="6" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="67" spans="2:5">
       <c r="B67" s="8" t="s">
@@ -2109,7 +2252,9 @@
       <c r="D67" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="6"/>
+      <c r="E67" s="6" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="8" t="s">
@@ -2121,7 +2266,9 @@
       <c r="D68" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E68" s="6"/>
+      <c r="E68" s="6" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="69" spans="2:5">
       <c r="B69" s="8" t="s">
@@ -2133,7 +2280,9 @@
       <c r="D69" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="6" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="8" t="s">
@@ -2146,7 +2295,7 @@
         <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2160,7 +2309,7 @@
         <v>93</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>129</v>
+        <v>296</v>
       </c>
     </row>
     <row r="72" spans="2:5">
@@ -2174,7 +2323,7 @@
         <v>93</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>130</v>
+        <v>297</v>
       </c>
     </row>
     <row r="73" spans="2:5">
@@ -2188,7 +2337,7 @@
         <v>93</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>131</v>
+        <v>298</v>
       </c>
     </row>
     <row r="74" spans="2:5">
@@ -2202,7 +2351,7 @@
         <v>93</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>132</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="30">
@@ -2276,7 +2425,7 @@
         <v>49</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="30">
@@ -2290,326 +2439,596 @@
         <v>49</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="30">
       <c r="B82" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E82" s="6"/>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>142</v>
-      </c>
       <c r="E83" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="30">
       <c r="B85" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="30">
       <c r="B86" s="8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E86" s="6"/>
     </row>
     <row r="87" spans="2:5" ht="30">
       <c r="B87" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="63.75" customHeight="1">
       <c r="B88" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="55.5" customHeight="1">
       <c r="B89" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="2:5" ht="78.75" customHeight="1">
       <c r="B93" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="60">
       <c r="B94" s="8" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="2:5" ht="30">
       <c r="B95" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E95" s="6"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="8" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C96" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E96" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="8" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="8" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E98" s="6"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="8" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E99" s="6"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="8" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E100" s="6"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="8" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E101" s="6"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E103" s="6"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="8" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="8" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="2:5" ht="30">
       <c r="B106" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="2:5" s="1" customFormat="1" ht="30">
+      <c r="B107" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" s="1" customFormat="1">
+      <c r="B108" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" s="1" customFormat="1">
+      <c r="B109" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" s="1" customFormat="1">
+      <c r="B110" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" s="1" customFormat="1" ht="33.75" customHeight="1">
+      <c r="B111" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C111" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" s="1" customFormat="1" ht="30.75" customHeight="1">
+      <c r="B112" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" s="1" customFormat="1">
+      <c r="B113" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="D106" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="E106" s="6"/>
+      <c r="C113" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" s="1" customFormat="1">
+      <c r="B114" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" s="1" customFormat="1">
+      <c r="B115" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5">
+      <c r="B116" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="2:5" ht="27" customHeight="1">
+      <c r="B117" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="2:5">
+      <c r="B118" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="2:5">
+      <c r="B119" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="2:5" ht="32.25" customHeight="1">
+      <c r="B120" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="2:5">
+      <c r="B121" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="2:5">
+      <c r="B122" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="2:5">
+      <c r="B123" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="2:5">
+      <c r="B124" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="2:5">
+      <c r="B125" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="2:5">
+      <c r="B126" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="2:5">
+      <c r="B127" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E127" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added updated carbon-climate conformance docs
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@840 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="313">
   <si>
     <t>ID</t>
   </si>
@@ -480,15 +480,9 @@
     <t>1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
   </si>
   <si>
-    <t>3.1S_100yrControl</t>
-  </si>
-  <si>
     <t>6.2a.HansenBaseline; 3.1S_100yrControl</t>
   </si>
   <si>
-    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl</t>
-  </si>
-  <si>
     <t>ic.008</t>
   </si>
   <si>
@@ -630,9 +624,6 @@
     <t>6.2b.Hansen4XCO2.xml; 6.5.CloudResponse.4CO2</t>
   </si>
   <si>
-    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl; 6.5.CloudResponse.4CO2</t>
-  </si>
-  <si>
     <t>3.3E_AMIP_Ensemble; 6.5.CloudResponse.4CO2</t>
   </si>
   <si>
@@ -753,9 +744,6 @@
     <t>Impose last glacial maximum ice sheet conditions supplied by PMIP</t>
   </si>
   <si>
-    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.4_MidHolocene; 3.5_Last_Glacial_Max; 3.6_Last_Millennium</t>
-  </si>
-  <si>
     <t>bc.074</t>
   </si>
   <si>
@@ -934,6 +922,39 @@
   </si>
   <si>
     <t>4.1L.RCP4.5_Ext</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength</t>
+  </si>
+  <si>
+    <t>bc.097</t>
+  </si>
+  <si>
+    <t>bc.098</t>
+  </si>
+  <si>
+    <t>5.4_Feedback_Strength</t>
+  </si>
+  <si>
+    <t>Forced with prescribed CO2 concentrations following either (1) spin off from the control (expt. 3.1) at the same point as expt. 6.1 and impose conditions identical to the control except that the carbon cycle 'sees' atmospheric CO2 concentration increase at a rate of 1%/yr (as in expt. 6.1)or ( 2) spin off from the control (expt. 3.1) at the same point as expt. 3.2 and impose conditions identical to the control except that the carbon cycle 'sees' increasing atmospheric CO2 concentrations that are identical to those prescribed in expt. 3.2 (for the historical period) and expt. 4.1 (RCP4.5 for the future). For both only the carbon cycle 'sees'  the CO2 increase</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.4_MidHolocene; 3.5_Last_Glacial_Max; 3.6_Last_Millennium; 5.4_Feedback_Strength; 5.5_rad_co2inc</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl; 5.4_Feedback_Strength; ; 5.5_rad_co2inc</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength; 5.5_rad_co2inc</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl; 6.5.CloudResponse.4CO2; 5.4_Feedback_Strength; ; 5.5_rad_co2inc</t>
+  </si>
+  <si>
+    <t>5.5_rad_co2inc</t>
+  </si>
+  <si>
+    <t>Forced with prescribed CO2 concentrations following either (1) spin off from the control (expt. 3.1) at the same point as expt. 6.1 and impose conditions identical to the control except that the carbon cycle 'sees' atmospheric CO2 concentration increase at a rate of 1%/yr (as in expt. 6.1)or ( 2) spin off from the control (expt. 3.1) at the same point as expt. 3.2 and impose conditions identical to the control except that only the radiation code 'sees' increasing atmospheric CO2 concentrations that are identical to those prescribed in expt. 3.2 (for the historical period) and expt. 4.1 (RCP4.5 for the future). For both the carbon cycle responds to the climate change alone</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1076,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1082,6 +1103,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1380,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G127"/>
+  <dimension ref="B2:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1431,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>245</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="53.25" customHeight="1">
@@ -1445,7 +1469,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -1462,7 +1486,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="36.75" customHeight="1">
@@ -1476,7 +1500,7 @@
         <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="28.5" customHeight="1">
@@ -1519,22 +1543,22 @@
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1">
       <c r="B11" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:7" ht="30">
       <c r="B12" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>147</v>
@@ -1543,10 +1567,10 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>152</v>
@@ -1555,145 +1579,145 @@
     </row>
     <row r="14" spans="2:7" ht="30">
       <c r="B14" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="2:7" ht="45">
       <c r="B16" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="2:7" ht="30">
       <c r="B18" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="2:7" ht="30">
       <c r="B19" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="2:7" ht="30">
       <c r="B20" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:7" s="1" customFormat="1" ht="32.25" customHeight="1">
       <c r="B21" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="36" customHeight="1">
       <c r="B22" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="30">
       <c r="B23" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E25" s="6"/>
     </row>
@@ -1754,7 +1778,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>154</v>
+        <v>308</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>45</v>
@@ -1771,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30">
@@ -1785,7 +1809,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>154</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="2:7">
@@ -1799,10 +1823,10 @@
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="41.25" customHeight="1">
       <c r="B36" s="8" t="s">
         <v>13</v>
       </c>
@@ -1813,7 +1837,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>154</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="30">
@@ -1827,7 +1851,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>154</v>
+        <v>308</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>29</v>
@@ -1844,7 +1868,7 @@
         <v>6</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>156</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30">
@@ -1858,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>156</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30">
@@ -1872,13 +1896,13 @@
         <v>6</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>156</v>
+        <v>309</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="30">
+    <row r="41" spans="2:7" ht="58.5" customHeight="1">
       <c r="B41" s="8" t="s">
         <v>18</v>
       </c>
@@ -1889,7 +1913,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="119.25" customHeight="1">
@@ -1903,7 +1927,7 @@
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="123" customHeight="1">
@@ -1917,7 +1941,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="120" customHeight="1">
@@ -1931,7 +1955,7 @@
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="120.75" customHeight="1">
@@ -1945,7 +1969,7 @@
         <v>49</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="111.75" customHeight="1">
@@ -1959,7 +1983,7 @@
         <v>49</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="138" customHeight="1">
@@ -1973,7 +1997,7 @@
         <v>49</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="138" customHeight="1">
@@ -1987,7 +2011,7 @@
         <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="117.75" customHeight="1">
@@ -2001,7 +2025,7 @@
         <v>49</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="114.75" customHeight="1">
@@ -2015,7 +2039,7 @@
         <v>49</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="110.25" customHeight="1">
@@ -2029,7 +2053,7 @@
         <v>49</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="108.75" customHeight="1">
@@ -2043,7 +2067,7 @@
         <v>49</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="101.25" customHeight="1">
@@ -2057,7 +2081,7 @@
         <v>49</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="44.25" customHeight="1">
@@ -2071,7 +2095,7 @@
         <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="39.75" customHeight="1">
@@ -2085,7 +2109,7 @@
         <v>65</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="60">
@@ -2099,7 +2123,7 @@
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="90" customHeight="1">
@@ -2113,7 +2137,7 @@
         <v>72</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="2:5" ht="71.25" customHeight="1">
@@ -2127,7 +2151,7 @@
         <v>72</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="2:5" ht="75" customHeight="1">
@@ -2141,7 +2165,7 @@
         <v>72</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="79.5" customHeight="1">
@@ -2155,7 +2179,7 @@
         <v>72</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="2:5" ht="60">
@@ -2169,7 +2193,7 @@
         <v>72</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="75.75" customHeight="1">
@@ -2183,7 +2207,7 @@
         <v>72</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="2:5" ht="60">
@@ -2197,7 +2221,7 @@
         <v>72</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="67.5" customHeight="1">
@@ -2211,7 +2235,7 @@
         <v>72</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="79.5" customHeight="1">
@@ -2225,7 +2249,7 @@
         <v>72</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="30">
@@ -2239,7 +2263,7 @@
         <v>93</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -2253,7 +2277,7 @@
         <v>93</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="2:5">
@@ -2267,7 +2291,7 @@
         <v>93</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="69" spans="2:5">
@@ -2281,7 +2305,7 @@
         <v>93</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -2295,7 +2319,7 @@
         <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2309,7 +2333,7 @@
         <v>93</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="2:5">
@@ -2323,7 +2347,7 @@
         <v>93</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="2:5">
@@ -2337,7 +2361,7 @@
         <v>93</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="2:5">
@@ -2351,7 +2375,7 @@
         <v>93</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="30">
@@ -2425,7 +2449,7 @@
         <v>49</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="30">
@@ -2439,7 +2463,7 @@
         <v>49</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="30">
@@ -2479,7 +2503,7 @@
         <v>136</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="30">
@@ -2493,7 +2517,7 @@
         <v>136</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="30">
@@ -2519,7 +2543,7 @@
         <v>141</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="63.75" customHeight="1">
@@ -2530,10 +2554,10 @@
         <v>149</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="55.5" customHeight="1">
@@ -2544,491 +2568,515 @@
         <v>151</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D92" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="2:5" ht="78.75" customHeight="1">
       <c r="B93" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>185</v>
-      </c>
       <c r="D93" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="60">
       <c r="B94" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D94" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="E94" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="2:5" ht="30">
       <c r="B95" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E95" s="6"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E98" s="6"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E99" s="6"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C100" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="D100" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E100" s="6"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E101" s="6"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D103" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="E103" s="6"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>250</v>
-      </c>
       <c r="D105" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="2:5" ht="30">
       <c r="B106" s="8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="2:5" s="1" customFormat="1" ht="30">
       <c r="B107" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="108" spans="2:5" s="1" customFormat="1">
       <c r="B108" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" spans="2:5" s="1" customFormat="1">
       <c r="B109" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="110" spans="2:5" s="1" customFormat="1">
       <c r="B110" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="2:5" s="1" customFormat="1" ht="33.75" customHeight="1">
       <c r="B111" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="112" spans="2:5" s="1" customFormat="1" ht="30.75" customHeight="1">
       <c r="B112" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="113" spans="2:5" s="1" customFormat="1">
       <c r="B113" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>261</v>
-      </c>
       <c r="E113" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="114" spans="2:5" s="1" customFormat="1">
       <c r="B114" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="115" spans="2:5" s="1" customFormat="1">
       <c r="B115" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="116" spans="2:5">
       <c r="B116" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E116" s="6"/>
     </row>
     <row r="117" spans="2:5" ht="27" customHeight="1">
       <c r="B117" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E117" s="6"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E118" s="6"/>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E119" s="6"/>
     </row>
     <row r="120" spans="2:5" ht="32.25" customHeight="1">
       <c r="B120" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E120" s="6"/>
     </row>
     <row r="121" spans="2:5">
       <c r="B121" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C121" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D121" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="E121" s="6"/>
     </row>
     <row r="122" spans="2:5">
       <c r="B122" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E122" s="6"/>
     </row>
     <row r="123" spans="2:5">
       <c r="B123" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E123" s="6"/>
     </row>
     <row r="124" spans="2:5">
       <c r="B124" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E124" s="6"/>
     </row>
     <row r="125" spans="2:5">
       <c r="B125" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E125" s="6"/>
     </row>
     <row r="126" spans="2:5">
       <c r="B126" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E126" s="6"/>
     </row>
     <row r="127" spans="2:5">
       <c r="B127" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D127" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="2:5" ht="159.75" customHeight="1">
+      <c r="B128" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="E128" s="6"/>
+    </row>
+    <row r="129" spans="2:5" ht="181.5" customHeight="1">
+      <c r="B129" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="E127" s="6"/>
+      <c r="C129" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E129" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded remaining conformance docs and completed crossover spreadsheet
git-svn-id: http://proj.badc.rl.ac.uk/svn/metafor/cmip5q/trunk@843 4926d154-5f4e-0410-ae62-53d2c911a6ca
</commit_message>
<xml_diff>
--- a/cmip5q/cmip5q/data/experiments/Conformances.xlsx
+++ b/cmip5q/cmip5q/data/experiments/Conformances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="331">
   <si>
     <t>ID</t>
   </si>
@@ -480,9 +480,6 @@
     <t>1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial</t>
   </si>
   <si>
-    <t>6.2a.HansenBaseline; 3.1S_100yrControl</t>
-  </si>
-  <si>
     <t>ic.008</t>
   </si>
   <si>
@@ -618,9 +615,6 @@
     <t>Different initial conditions imposed on land surface to that of experiment 2.1</t>
   </si>
   <si>
-    <t>6.3.GregoryAbrupt4XCO2; 6.5.CloudResponse.4CO2</t>
-  </si>
-  <si>
     <t>6.2b.Hansen4XCO2.xml; 6.5.CloudResponse.4CO2</t>
   </si>
   <si>
@@ -681,9 +675,6 @@
     <t>6.8.Cloudresponse.UniSST</t>
   </si>
   <si>
-    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2; 3.2E_HistoricalEnsemble</t>
-  </si>
-  <si>
     <t>Additional runs, initialised at different points in the control run</t>
   </si>
   <si>
@@ -696,9 +687,6 @@
     <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.2E_HistoricalEnsemble</t>
   </si>
   <si>
-    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 3.2E_HistoricalEnsemble</t>
-  </si>
-  <si>
     <t>5.2.ESMHistoricalC20th; 3.2E_HistoricalEnsemble</t>
   </si>
   <si>
@@ -924,9 +912,6 @@
     <t>4.1L.RCP4.5_Ext</t>
   </si>
   <si>
-    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength</t>
-  </si>
-  <si>
     <t>bc.097</t>
   </si>
   <si>
@@ -939,22 +924,91 @@
     <t>Forced with prescribed CO2 concentrations following either (1) spin off from the control (expt. 3.1) at the same point as expt. 6.1 and impose conditions identical to the control except that the carbon cycle 'sees' atmospheric CO2 concentration increase at a rate of 1%/yr (as in expt. 6.1)or ( 2) spin off from the control (expt. 3.1) at the same point as expt. 3.2 and impose conditions identical to the control except that the carbon cycle 'sees' increasing atmospheric CO2 concentrations that are identical to those prescribed in expt. 3.2 (for the historical period) and expt. 4.1 (RCP4.5 for the future). For both only the carbon cycle 'sees'  the CO2 increase</t>
   </si>
   <si>
-    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.4_MidHolocene; 3.5_Last_Glacial_Max; 3.6_Last_Millennium; 5.4_Feedback_Strength; 5.5_rad_co2inc</t>
-  </si>
-  <si>
-    <t>3.1S_100yrControl; 5.4_Feedback_Strength; ; 5.5_rad_co2inc</t>
-  </si>
-  <si>
-    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength; 5.5_rad_co2inc</t>
-  </si>
-  <si>
-    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl; 6.5.CloudResponse.4CO2; 5.4_Feedback_Strength; ; 5.5_rad_co2inc</t>
-  </si>
-  <si>
     <t>5.5_rad_co2inc</t>
   </si>
   <si>
     <t>Forced with prescribed CO2 concentrations following either (1) spin off from the control (expt. 3.1) at the same point as expt. 6.1 and impose conditions identical to the control except that the carbon cycle 'sees' atmospheric CO2 concentration increase at a rate of 1%/yr (as in expt. 6.1)or ( 2) spin off from the control (expt. 3.1) at the same point as expt. 3.2 and impose conditions identical to the control except that only the radiation code 'sees' increasing atmospheric CO2 concentrations that are identical to those prescribed in expt. 3.2 (for the historical period) and expt. 4.1 (RCP4.5 for the future). For both the carbon cycle responds to the climate change alone</t>
+  </si>
+  <si>
+    <t>ic.023</t>
+  </si>
+  <si>
+    <t>Each of the 11 ensemble members must be initialised in a different month of the year</t>
+  </si>
+  <si>
+    <t>6.3E.Ensemble_Abrupt4XCO2</t>
+  </si>
+  <si>
+    <t>6.3.GregoryAbrupt4XCO2; 6.5.CloudResponse.4CO2; 6.3E.Ensemble_Abrupt4XCO2</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl, 2.1_FutureTimeSlice, 2.1E_FutureTimeSlice_Ensemble; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.4_MidHolocene; 3.5_Last_Glacial_Max; 3.6_Last_Millennium; 5.4_Feedback_Strength; 5.5_rad_co2inc; 6.3E.Ensemble_Abrupt4XCO2; 6.4.Hansen_Aerosol</t>
+  </si>
+  <si>
+    <t>bc.099</t>
+  </si>
+  <si>
+    <t>Aerosols should be consistant with year 2000 of the historical run (3.2)</t>
+  </si>
+  <si>
+    <t>6.4.Hansen_Aerosol</t>
+  </si>
+  <si>
+    <t>bc.100</t>
+  </si>
+  <si>
+    <t>Create multi-member ensembles initialised from different points in the control run</t>
+  </si>
+  <si>
+    <t>7.1E_NaturalOnly_Ensemble</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.2E_HistoricalEnsemble; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 6.7a.Aquaplanet_Control; 6.7b_Aquaplanet_4CO2; 6.7c_Aquaplanet_4K; 6.8.Cloudresponse.UniSST; 3.2E_HistoricalEnsemble; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly</t>
+  </si>
+  <si>
+    <t>3.3.AMIP; 5.2.ESMHistoricalC20th; 1.1_DecadalHindcast; 1.5_decadal_AlterInit; 1.4_2010Pinutubo; 1.2_30yrHindcast; 1.1E_DecadalHindcast_O10; 1.2E_30yrHindcast_O10; 1.1I_DecadalHindcast_Initial; 1.3.DecadalHindcast_NoVolc; 3.3E_AMIP_Ensemble; 6.6.CloudResponse.SST; 3.2E_HistoricalEnsemble; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly</t>
+  </si>
+  <si>
+    <t>5.2.ESMHistoricalC20th; 6.1.1pcto4XCO2; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2; 6.5.CloudResponse.4CO2; 3.2E_HistoricalEnsemble; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.2_GHGOnly</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 6.2a.HansenBaseline; 6.2b.Hansen4XCO2.xml; 3.1S_100yrControl; 6.5.CloudResponse.4CO2; 5.4_Feedback_Strength; ; 5.5_rad_co2inc; 6.4.Hansen_Aerosol; ; 7.2_GHGOnly</t>
+  </si>
+  <si>
+    <t>bc.101</t>
+  </si>
+  <si>
+    <t>Impose changing conditions of, for example, land use change only, anthropogenic aerosols only, or volcanic aerosols only etc</t>
+  </si>
+  <si>
+    <t>7.3E_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>7.2E_GHGOnly_Ensemble; 7.3E_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>7.3_OtherForcing</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl; 5.4_Feedback_Strength; ; 5.5_rad_co2inc; 6.4.Hansen_Aerosol; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>6.2a.HansenBaseline; 3.1S_100yrControl; 6.4.Hansen_Aerosol; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl; 5.4_Feedback_Strength; ; 5.5_rad_co2inc; 6.4.Hansen_Aerosol; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.2_GHGOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>3.1S_100yrControl; 5.4_Feedback_Strength; ; 5.5_rad_co2inc; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.2_GHGOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.2_GHGOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
+  </si>
+  <si>
+    <t>5.1.ESMPreIndustrialControl; 3.1S_100yrControl; 5.4_Feedback_Strength; 5.5_rad_co2inc; 7.1E_NaturalOnly_Ensemble; 7.1_NaturalOnly; 7.2_GHGOnly; 7.3_OtherForcing; 7.3_OtherForcing_Ensemble</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G129"/>
+  <dimension ref="B2:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -1455,10 +1509,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="53.25" customHeight="1">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="65.25" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
@@ -1469,7 +1523,7 @@
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>221</v>
+        <v>318</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -1486,7 +1540,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="36.75" customHeight="1">
@@ -1500,7 +1554,7 @@
         <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="28.5" customHeight="1">
@@ -1543,22 +1597,22 @@
     </row>
     <row r="11" spans="2:7" ht="31.5" customHeight="1">
       <c r="B11" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>157</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="2:7" ht="30">
       <c r="B12" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>147</v>
@@ -1567,10 +1621,10 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>152</v>
@@ -1579,152 +1633,158 @@
     </row>
     <row r="14" spans="2:7" ht="30">
       <c r="B14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="D15" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="2:7" ht="45">
       <c r="B16" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>179</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="2:7" ht="30">
       <c r="B18" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="2:7" ht="30">
       <c r="B19" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="2:7" ht="30">
       <c r="B20" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="2:7" s="1" customFormat="1" ht="32.25" customHeight="1">
       <c r="B21" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="2:7" ht="36" customHeight="1">
       <c r="B22" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="2:7" ht="30">
       <c r="B23" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>239</v>
-      </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="12"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+    <row r="26" spans="2:7" ht="30">
+      <c r="B26" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>306</v>
+      </c>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="2:7">
@@ -1767,7 +1827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30.75" thickTop="1">
+    <row r="32" spans="2:7" ht="61.5" customHeight="1" thickTop="1">
       <c r="B32" s="8" t="s">
         <v>9</v>
       </c>
@@ -1778,13 +1838,13 @@
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30">
+    <row r="33" spans="2:7" ht="45">
       <c r="B33" s="8" t="s">
         <v>10</v>
       </c>
@@ -1795,10 +1855,10 @@
         <v>6</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="45">
       <c r="B34" s="8" t="s">
         <v>11</v>
       </c>
@@ -1809,10 +1869,10 @@
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="45">
       <c r="B35" s="8" t="s">
         <v>12</v>
       </c>
@@ -1823,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="41.25" customHeight="1">
@@ -1837,10 +1897,10 @@
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="45">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -1851,13 +1911,13 @@
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" ht="60" customHeight="1">
       <c r="B38" s="8" t="s">
         <v>15</v>
       </c>
@@ -1868,10 +1928,10 @@
         <v>6</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="48" customHeight="1">
       <c r="B39" s="8" t="s">
         <v>16</v>
       </c>
@@ -1882,10 +1942,10 @@
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="30">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="45" customHeight="1">
       <c r="B40" s="8" t="s">
         <v>17</v>
       </c>
@@ -1896,7 +1956,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>29</v>
@@ -1913,7 +1973,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="119.25" customHeight="1">
@@ -1927,7 +1987,7 @@
         <v>49</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="123" customHeight="1">
@@ -1941,7 +2001,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>224</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="120" customHeight="1">
@@ -1955,7 +2015,7 @@
         <v>49</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="120.75" customHeight="1">
@@ -1969,7 +2029,7 @@
         <v>49</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="111.75" customHeight="1">
@@ -1983,7 +2043,7 @@
         <v>49</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="2:7" ht="138" customHeight="1">
@@ -1997,7 +2057,7 @@
         <v>49</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="138" customHeight="1">
@@ -2011,7 +2071,7 @@
         <v>49</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="117.75" customHeight="1">
@@ -2025,7 +2085,7 @@
         <v>49</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="114.75" customHeight="1">
@@ -2039,7 +2099,7 @@
         <v>49</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="110.25" customHeight="1">
@@ -2053,10 +2113,10 @@
         <v>49</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="108.75" customHeight="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="126.75" customHeight="1">
       <c r="B52" s="8" t="s">
         <v>55</v>
       </c>
@@ -2067,10 +2127,10 @@
         <v>49</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="101.25" customHeight="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="107.25" customHeight="1">
       <c r="B53" s="8" t="s">
         <v>56</v>
       </c>
@@ -2081,7 +2141,7 @@
         <v>49</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>226</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="44.25" customHeight="1">
@@ -2095,7 +2155,7 @@
         <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="39.75" customHeight="1">
@@ -2109,7 +2169,7 @@
         <v>65</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="60">
@@ -2123,7 +2183,7 @@
         <v>72</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="90" customHeight="1">
@@ -2137,7 +2197,7 @@
         <v>72</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="2:5" ht="71.25" customHeight="1">
@@ -2151,7 +2211,7 @@
         <v>72</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="2:5" ht="75" customHeight="1">
@@ -2165,7 +2225,7 @@
         <v>72</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="79.5" customHeight="1">
@@ -2179,7 +2239,7 @@
         <v>72</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" spans="2:5" ht="60">
@@ -2193,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="75.75" customHeight="1">
@@ -2207,7 +2267,7 @@
         <v>72</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="2:5" ht="60">
@@ -2221,7 +2281,7 @@
         <v>72</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="67.5" customHeight="1">
@@ -2235,7 +2295,7 @@
         <v>72</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="79.5" customHeight="1">
@@ -2249,7 +2309,7 @@
         <v>72</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="30">
@@ -2263,7 +2323,7 @@
         <v>93</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="2:5">
@@ -2277,7 +2337,7 @@
         <v>93</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="68" spans="2:5">
@@ -2291,7 +2351,7 @@
         <v>93</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="69" spans="2:5">
@@ -2305,7 +2365,7 @@
         <v>93</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="2:5">
@@ -2319,7 +2379,7 @@
         <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="2:5">
@@ -2333,7 +2393,7 @@
         <v>93</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="2:5">
@@ -2347,7 +2407,7 @@
         <v>93</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="2:5">
@@ -2361,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="2:5">
@@ -2375,7 +2435,7 @@
         <v>93</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="30">
@@ -2449,7 +2509,7 @@
         <v>49</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="30">
@@ -2463,7 +2523,7 @@
         <v>49</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="30">
@@ -2503,7 +2563,7 @@
         <v>136</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="2:5" ht="30">
@@ -2517,7 +2577,7 @@
         <v>136</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="30">
@@ -2543,7 +2603,7 @@
         <v>141</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>200</v>
+        <v>307</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="63.75" customHeight="1">
@@ -2554,10 +2614,10 @@
         <v>149</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="55.5" customHeight="1">
@@ -2568,515 +2628,555 @@
         <v>151</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="B90" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="D90" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="D91" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="D92" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="2:5" ht="78.75" customHeight="1">
       <c r="B93" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C93" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D93" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D93" s="8" t="s">
-        <v>184</v>
-      </c>
       <c r="E93" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="60">
       <c r="B94" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="2:5" ht="30">
       <c r="B95" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D95" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="E95" s="6"/>
     </row>
     <row r="96" spans="2:5">
       <c r="B96" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>210</v>
-      </c>
       <c r="E96" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="2:5">
       <c r="B97" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="2:5">
       <c r="B98" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="E98" s="6"/>
     </row>
     <row r="99" spans="2:5">
       <c r="B99" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D99" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="E99" s="6"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E100" s="6"/>
     </row>
     <row r="101" spans="2:5">
       <c r="B101" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E101" s="6"/>
     </row>
     <row r="102" spans="2:5">
       <c r="B102" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E103" s="6"/>
     </row>
     <row r="104" spans="2:5">
       <c r="B104" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C104" s="6" t="s">
-        <v>241</v>
-      </c>
       <c r="D104" s="8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C105" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="D105" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="2:5" ht="30">
       <c r="B106" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="2:5" s="1" customFormat="1" ht="30">
       <c r="B107" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="2:5" s="1" customFormat="1">
       <c r="B108" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="109" spans="2:5" s="1" customFormat="1">
       <c r="B109" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="110" spans="2:5" s="1" customFormat="1">
       <c r="B110" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" spans="2:5" s="1" customFormat="1" ht="33.75" customHeight="1">
       <c r="B111" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="112" spans="2:5" s="1" customFormat="1" ht="30.75" customHeight="1">
       <c r="B112" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" spans="2:5" s="1" customFormat="1">
       <c r="B113" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="E113" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="114" spans="2:5" s="1" customFormat="1">
       <c r="B114" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="115" spans="2:5" s="1" customFormat="1">
       <c r="B115" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="116" spans="2:5">
       <c r="B116" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E116" s="6"/>
     </row>
     <row r="117" spans="2:5" ht="27" customHeight="1">
       <c r="B117" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E117" s="6"/>
     </row>
     <row r="118" spans="2:5">
       <c r="B118" s="6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E118" s="6"/>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E119" s="6"/>
     </row>
     <row r="120" spans="2:5" ht="32.25" customHeight="1">
       <c r="B120" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E120" s="6"/>
     </row>
     <row r="121" spans="2:5">
       <c r="B121" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C121" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D121" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="E121" s="6"/>
     </row>
     <row r="122" spans="2:5">
       <c r="B122" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E122" s="6"/>
     </row>
     <row r="123" spans="2:5">
       <c r="B123" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E123" s="6"/>
     </row>
     <row r="124" spans="2:5">
       <c r="B124" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E124" s="6"/>
     </row>
     <row r="125" spans="2:5">
       <c r="B125" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E125" s="6"/>
     </row>
     <row r="126" spans="2:5">
       <c r="B126" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E126" s="6"/>
     </row>
     <row r="127" spans="2:5">
       <c r="B127" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E127" s="6"/>
     </row>
     <row r="128" spans="2:5" ht="159.75" customHeight="1">
       <c r="B128" s="6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E128" s="6"/>
     </row>
     <row r="129" spans="2:5" ht="181.5" customHeight="1">
       <c r="B129" s="6" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C129" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E129" s="6"/>
+    </row>
+    <row r="130" spans="2:5" ht="34.5" customHeight="1">
+      <c r="B130" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="2:5" ht="30">
+      <c r="B131" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D129" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E129" s="6"/>
+      <c r="C131" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="30">
+      <c r="B132" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>322</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>